<commit_message>
added another sheet to the zip code workbook and changed the file that the scraper checks to see if the data's been updated, since the zip code data has not been updated for 2 days now. -M
</commit_message>
<xml_diff>
--- a/zip code positivity rate data.xlsx
+++ b/zip code positivity rate data.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://caltech-my.sharepoint.com/personal/mrupprec_caltech_edu/Documents/Documents/musings, et cetera/COVID-19/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{28F728B8-2643-446C-A6B8-CFE20971D646}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="10" documentId="8_{28F728B8-2643-446C-A6B8-CFE20971D646}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{DAD8FB44-430C-4D33-9EF4-EC99BF8B7E6A}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{7664FA99-CE0E-4C3D-8047-C7C230C2EB15}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{7664FA99-CE0E-4C3D-8047-C7C230C2EB15}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -34,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="13">
   <si>
     <t>total</t>
   </si>
@@ -70,6 +71,9 @@
   </si>
   <si>
     <t>data from 7/09 to 7/20</t>
+  </si>
+  <si>
+    <t>data from 9/29 to 10/10</t>
   </si>
 </sst>
 </file>
@@ -423,8 +427,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F27300E4-DFF6-4EC7-9A51-39706208D925}">
   <dimension ref="A1:F19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I23" sqref="I23"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D29" sqref="D29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -791,4 +795,375 @@
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{293184C4-EBDF-4BB1-AC48-B163FE25A774}">
+  <dimension ref="A1:F19"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E10" sqref="E10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A2">
+        <v>60631</v>
+      </c>
+      <c r="B2">
+        <v>4.7</v>
+      </c>
+      <c r="C2">
+        <v>6.5</v>
+      </c>
+      <c r="D2">
+        <f>LN(C2/B2)</f>
+        <v>0.32423966818557842</v>
+      </c>
+      <c r="E2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A3">
+        <v>60656</v>
+      </c>
+      <c r="B3">
+        <v>7.8</v>
+      </c>
+      <c r="C3">
+        <v>10.4</v>
+      </c>
+      <c r="D3">
+        <f t="shared" ref="D3:D18" si="0">LN(C3/B3)</f>
+        <v>0.28768207245178101</v>
+      </c>
+      <c r="E3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A4">
+        <v>60706</v>
+      </c>
+      <c r="B4">
+        <v>5.5</v>
+      </c>
+      <c r="C4">
+        <v>9.8000000000000007</v>
+      </c>
+      <c r="D4">
+        <f t="shared" si="0"/>
+        <v>0.57763429343810113</v>
+      </c>
+      <c r="E4" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A5">
+        <v>60634</v>
+      </c>
+      <c r="B5">
+        <v>6.7</v>
+      </c>
+      <c r="C5">
+        <v>6.3</v>
+      </c>
+      <c r="D5">
+        <f t="shared" si="0"/>
+        <v>-6.1557892999433435E-2</v>
+      </c>
+      <c r="E5" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A6">
+        <v>60714</v>
+      </c>
+      <c r="B6">
+        <v>4.0999999999999996</v>
+      </c>
+      <c r="C6">
+        <v>9</v>
+      </c>
+      <c r="D6">
+        <f t="shared" si="0"/>
+        <v>0.78623760362595729</v>
+      </c>
+      <c r="E6" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A7">
+        <v>60053</v>
+      </c>
+      <c r="B7">
+        <v>3.4</v>
+      </c>
+      <c r="C7">
+        <v>5.0999999999999996</v>
+      </c>
+      <c r="D7">
+        <f t="shared" si="0"/>
+        <v>0.40546510810816438</v>
+      </c>
+      <c r="E7" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A8">
+        <v>60077</v>
+      </c>
+      <c r="B8">
+        <v>0.9</v>
+      </c>
+      <c r="C8">
+        <v>1.2</v>
+      </c>
+      <c r="D8">
+        <f t="shared" si="0"/>
+        <v>0.28768207245178085</v>
+      </c>
+      <c r="E8" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A9">
+        <v>60076</v>
+      </c>
+      <c r="B9">
+        <v>5.6</v>
+      </c>
+      <c r="C9">
+        <v>5.7</v>
+      </c>
+      <c r="D9">
+        <f t="shared" si="0"/>
+        <v>1.7699577099401075E-2</v>
+      </c>
+      <c r="E9" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A10">
+        <v>60203</v>
+      </c>
+      <c r="B10">
+        <v>3.9</v>
+      </c>
+      <c r="C10">
+        <v>4</v>
+      </c>
+      <c r="D10">
+        <f t="shared" si="0"/>
+        <v>2.5317807984290001E-2</v>
+      </c>
+      <c r="E10" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A11">
+        <v>60712</v>
+      </c>
+      <c r="B11">
+        <v>3.4</v>
+      </c>
+      <c r="C11">
+        <v>1.8</v>
+      </c>
+      <c r="D11">
+        <f t="shared" si="0"/>
+        <v>-0.63598876671999671</v>
+      </c>
+      <c r="E11" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A12">
+        <v>60646</v>
+      </c>
+      <c r="B12">
+        <v>3.4</v>
+      </c>
+      <c r="C12">
+        <v>4.5999999999999996</v>
+      </c>
+      <c r="D12">
+        <f t="shared" si="0"/>
+        <v>0.30228087187293351</v>
+      </c>
+      <c r="E12" t="s">
+        <v>5</v>
+      </c>
+      <c r="F12" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A13">
+        <v>60630</v>
+      </c>
+      <c r="B13">
+        <v>6.3</v>
+      </c>
+      <c r="C13">
+        <v>5.4</v>
+      </c>
+      <c r="D13">
+        <f t="shared" si="0"/>
+        <v>-0.15415067982725822</v>
+      </c>
+      <c r="E13" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A14">
+        <v>60641</v>
+      </c>
+      <c r="B14">
+        <v>4.8</v>
+      </c>
+      <c r="C14">
+        <v>3.4</v>
+      </c>
+      <c r="D14">
+        <f t="shared" si="0"/>
+        <v>-0.34484048629172948</v>
+      </c>
+      <c r="E14" t="s">
+        <v>3</v>
+      </c>
+      <c r="F14" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A15">
+        <v>60645</v>
+      </c>
+      <c r="B15">
+        <v>2.8</v>
+      </c>
+      <c r="C15">
+        <v>4.8</v>
+      </c>
+      <c r="D15">
+        <f t="shared" si="0"/>
+        <v>0.53899650073268712</v>
+      </c>
+      <c r="E15" t="s">
+        <v>3</v>
+      </c>
+      <c r="F15" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A16">
+        <v>60659</v>
+      </c>
+      <c r="B16">
+        <v>6.3</v>
+      </c>
+      <c r="C16">
+        <v>9.1</v>
+      </c>
+      <c r="D16">
+        <f t="shared" si="0"/>
+        <v>0.36772478012531734</v>
+      </c>
+      <c r="E16" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A17">
+        <v>60625</v>
+      </c>
+      <c r="B17">
+        <v>4.5</v>
+      </c>
+      <c r="C17">
+        <v>4.0999999999999996</v>
+      </c>
+      <c r="D17">
+        <f t="shared" si="0"/>
+        <v>-9.309042306601209E-2</v>
+      </c>
+      <c r="E17" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A18">
+        <v>60618</v>
+      </c>
+      <c r="B18">
+        <v>3.9</v>
+      </c>
+      <c r="C18">
+        <v>2.5</v>
+      </c>
+      <c r="D18">
+        <f t="shared" si="0"/>
+        <v>-0.44468582126144557</v>
+      </c>
+      <c r="E18" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B19" t="s">
+        <v>12</v>
+      </c>
+    </row>
+  </sheetData>
+  <conditionalFormatting sqref="D2:D18">
+    <cfRule type="colorScale" priority="2">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="num" val="0"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B2:C18">
+    <cfRule type="colorScale" priority="1">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>